<commit_message>
model change: now a physical model with flexible cops is introduced and a heat pump efficiency as a quality is added
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Configuration</t>
   </si>
   <si>
-    <t>building category</t>
-  </si>
-  <si>
     <t>[m]</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>floor area</t>
   </si>
   <si>
-    <t>[SIA category]</t>
-  </si>
-  <si>
     <t>altitude</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>air, radiator, floor heating, ceiling heating</t>
   </si>
   <si>
-    <t>cold emission</t>
-  </si>
-  <si>
     <t>PV type</t>
   </si>
   <si>
@@ -225,6 +216,27 @@
   </si>
   <si>
     <t>increased ventilation volume flow</t>
+  </si>
+  <si>
+    <t>105 30</t>
+  </si>
+  <si>
+    <t>26 25</t>
+  </si>
+  <si>
+    <t>180 120</t>
+  </si>
+  <si>
+    <t>cold emission system</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>radiator</t>
+  </si>
+  <si>
+    <t>heat pump efficiency</t>
   </si>
 </sst>
 </file>
@@ -552,27 +564,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="7" width="22.453125" customWidth="1"/>
-    <col min="8" max="10" width="17.6328125" customWidth="1"/>
-    <col min="11" max="11" width="34" customWidth="1"/>
-    <col min="12" max="14" width="14.1796875" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" customWidth="1"/>
-    <col min="16" max="16" width="16.54296875" customWidth="1"/>
-    <col min="17" max="17" width="64.1796875" customWidth="1"/>
-    <col min="18" max="18" width="16.36328125" customWidth="1"/>
-    <col min="19" max="25" width="21" customWidth="1"/>
-    <col min="26" max="26" width="21.90625" customWidth="1"/>
-    <col min="27" max="29" width="42.90625" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" customWidth="1"/>
+    <col min="5" max="6" width="22.453125" customWidth="1"/>
+    <col min="7" max="9" width="17.6328125" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
+    <col min="11" max="13" width="14.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" customWidth="1"/>
+    <col min="16" max="16" width="64.1796875" customWidth="1"/>
+    <col min="17" max="17" width="16.36328125" customWidth="1"/>
+    <col min="18" max="24" width="21" customWidth="1"/>
+    <col min="25" max="25" width="21.90625" customWidth="1"/>
+    <col min="26" max="29" width="42.90625" customWidth="1"/>
     <col min="30" max="31" width="14.36328125" customWidth="1"/>
     <col min="34" max="34" width="13" customWidth="1"/>
     <col min="35" max="35" width="20.1796875" customWidth="1"/>
@@ -585,70 +597,70 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
       </c>
       <c r="O1" t="s">
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="T1" t="s">
         <v>31</v>
       </c>
       <c r="U1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="X1" t="s">
         <v>35</v>
@@ -657,135 +669,135 @@
         <v>36</v>
       </c>
       <c r="Z1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>23</v>
-      </c>
       <c r="AK1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W2" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="X2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="AA2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD2" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>53</v>
-      </c>
       <c r="AH2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AK2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -793,91 +805,91 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1.1000000000000001</v>
+        <v>520</v>
       </c>
       <c r="C3" s="1">
-        <v>520</v>
+        <v>0.215</v>
       </c>
       <c r="D3" s="1">
-        <v>0.215</v>
+        <v>0.15</v>
       </c>
       <c r="E3" s="1">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="J3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1">
         <v>0.13</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="M3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>42</v>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1">
+        <v>137</v>
       </c>
       <c r="X3" s="1">
         <v>137</v>
       </c>
       <c r="Y3" s="1">
-        <v>137</v>
-      </c>
-      <c r="Z3" s="1">
         <v>435</v>
       </c>
+      <c r="Z3" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="AA3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>105</v>
-      </c>
       <c r="AG3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AH3" s="2">
         <v>0.18</v>
@@ -885,11 +897,11 @@
       <c r="AI3" s="2">
         <v>0.8</v>
       </c>
-      <c r="AJ3" s="2">
-        <v>180</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>26</v>
+      <c r="AJ3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
new input file order
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Configuration</t>
   </si>
   <si>
-    <t>building category</t>
-  </si>
-  <si>
     <t>[m]</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>floor area</t>
   </si>
   <si>
-    <t>[SIA category]</t>
-  </si>
-  <si>
     <t>altitude</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>air, radiator, floor heating, ceiling heating</t>
   </si>
   <si>
-    <t>cold emission</t>
-  </si>
-  <si>
     <t>PV type</t>
   </si>
   <si>
@@ -225,6 +216,27 @@
   </si>
   <si>
     <t>increased ventilation volume flow</t>
+  </si>
+  <si>
+    <t>105 30</t>
+  </si>
+  <si>
+    <t>26 25</t>
+  </si>
+  <si>
+    <t>180 120</t>
+  </si>
+  <si>
+    <t>cold emission system</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>radiator</t>
+  </si>
+  <si>
+    <t>heat pump efficiency</t>
   </si>
 </sst>
 </file>
@@ -552,27 +564,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="7" width="22.453125" customWidth="1"/>
-    <col min="8" max="10" width="17.6328125" customWidth="1"/>
-    <col min="11" max="11" width="34" customWidth="1"/>
-    <col min="12" max="14" width="14.1796875" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" customWidth="1"/>
-    <col min="16" max="16" width="16.54296875" customWidth="1"/>
-    <col min="17" max="17" width="64.1796875" customWidth="1"/>
-    <col min="18" max="18" width="16.36328125" customWidth="1"/>
-    <col min="19" max="25" width="21" customWidth="1"/>
-    <col min="26" max="26" width="21.90625" customWidth="1"/>
-    <col min="27" max="29" width="42.90625" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" customWidth="1"/>
+    <col min="5" max="6" width="22.453125" customWidth="1"/>
+    <col min="7" max="9" width="17.6328125" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
+    <col min="11" max="13" width="14.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" customWidth="1"/>
+    <col min="16" max="16" width="64.1796875" customWidth="1"/>
+    <col min="17" max="17" width="16.36328125" customWidth="1"/>
+    <col min="18" max="24" width="21" customWidth="1"/>
+    <col min="25" max="25" width="21.90625" customWidth="1"/>
+    <col min="26" max="29" width="42.90625" customWidth="1"/>
     <col min="30" max="31" width="14.36328125" customWidth="1"/>
     <col min="34" max="34" width="13" customWidth="1"/>
     <col min="35" max="35" width="20.1796875" customWidth="1"/>
@@ -585,70 +597,70 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
       </c>
       <c r="O1" t="s">
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="T1" t="s">
         <v>31</v>
       </c>
       <c r="U1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="X1" t="s">
         <v>35</v>
@@ -657,135 +669,135 @@
         <v>36</v>
       </c>
       <c r="Z1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>23</v>
-      </c>
       <c r="AK1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W2" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="X2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="AA2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD2" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>53</v>
-      </c>
       <c r="AH2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AJ2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AK2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -793,91 +805,91 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1.1000000000000001</v>
+        <v>520</v>
       </c>
       <c r="C3" s="1">
-        <v>520</v>
+        <v>0.215</v>
       </c>
       <c r="D3" s="1">
-        <v>0.215</v>
+        <v>0.15</v>
       </c>
       <c r="E3" s="1">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="J3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1">
         <v>0.13</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="M3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>42</v>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1">
+        <v>137</v>
       </c>
       <c r="X3" s="1">
         <v>137</v>
       </c>
       <c r="Y3" s="1">
-        <v>137</v>
-      </c>
-      <c r="Z3" s="1">
         <v>435</v>
       </c>
+      <c r="Z3" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="AA3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>105</v>
-      </c>
       <c r="AG3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AH3" s="2">
         <v>0.18</v>
@@ -885,11 +897,11 @@
       <c r="AI3" s="2">
         <v>0.8</v>
       </c>
-      <c r="AJ3" s="2">
-        <v>180</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>26</v>
+      <c r="AJ3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
it is now possible to have DHW without a room heating system, however if both is present, it needs to be the same.
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>Configuration</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>heat pump efficiency</t>
+  </si>
+  <si>
+    <t>dhw heating system</t>
+  </si>
+  <si>
+    <t>"same" or the choices from heating system</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK121"/>
+  <dimension ref="A1:AL121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,15 +590,15 @@
     <col min="17" max="17" width="16.36328125" customWidth="1"/>
     <col min="18" max="24" width="21" customWidth="1"/>
     <col min="25" max="25" width="21.90625" customWidth="1"/>
-    <col min="26" max="29" width="42.90625" customWidth="1"/>
-    <col min="30" max="31" width="14.36328125" customWidth="1"/>
-    <col min="34" max="34" width="13" customWidth="1"/>
-    <col min="35" max="35" width="20.1796875" customWidth="1"/>
-    <col min="36" max="36" width="18.81640625" customWidth="1"/>
-    <col min="37" max="37" width="16.6328125" customWidth="1"/>
+    <col min="26" max="30" width="42.90625" customWidth="1"/>
+    <col min="31" max="32" width="14.36328125" customWidth="1"/>
+    <col min="35" max="35" width="13" customWidth="1"/>
+    <col min="36" max="36" width="20.1796875" customWidth="1"/>
+    <col min="37" max="37" width="18.81640625" customWidth="1"/>
+    <col min="38" max="38" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,40 +678,43 @@
         <v>18</v>
       </c>
       <c r="AA1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>70</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>67</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>38</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>22</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -767,40 +776,43 @@
         <v>19</v>
       </c>
       <c r="AA2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>15</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>47</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>3</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>50</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>15</v>
       </c>
       <c r="AI2" t="s">
         <v>15</v>
       </c>
       <c r="AJ2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK2" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -868,55 +880,58 @@
         <v>435</v>
       </c>
       <c r="Z3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AI3" s="2">
         <v>0.18</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AJ3" s="2">
         <v>0.8</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
removed coulmns that do not affect simulation outcome. Further columns for data analysis can always be added
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>Configuration</t>
   </si>
@@ -119,12 +119,6 @@
     <t>wall areas</t>
   </si>
   <si>
-    <t>wall orientations</t>
-  </si>
-  <si>
-    <t>[doesn't matter ATM]</t>
-  </si>
-  <si>
     <t>[m2, m2, m2,…]</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t>N E S W</t>
   </si>
   <si>
-    <t>envelope type</t>
-  </si>
-  <si>
     <t>wall type</t>
   </si>
   <si>
@@ -186,12 +177,6 @@
   </si>
   <si>
     <t>UBA_EnEV_window</t>
-  </si>
-  <si>
-    <t>base material</t>
-  </si>
-  <si>
-    <t>wood/concrete</t>
   </si>
   <si>
     <t>UBA_all_stb</t>
@@ -568,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL121"/>
+  <dimension ref="A1:AI121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,24 +566,24 @@
     <col min="3" max="3" width="30.90625" customWidth="1"/>
     <col min="4" max="4" width="23.453125" customWidth="1"/>
     <col min="5" max="6" width="22.453125" customWidth="1"/>
-    <col min="7" max="9" width="17.6328125" customWidth="1"/>
-    <col min="10" max="10" width="34" customWidth="1"/>
-    <col min="11" max="13" width="14.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.54296875" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" customWidth="1"/>
-    <col min="16" max="16" width="64.1796875" customWidth="1"/>
-    <col min="17" max="17" width="16.36328125" customWidth="1"/>
-    <col min="18" max="24" width="21" customWidth="1"/>
-    <col min="25" max="25" width="21.90625" customWidth="1"/>
-    <col min="26" max="30" width="42.90625" customWidth="1"/>
-    <col min="31" max="32" width="14.36328125" customWidth="1"/>
-    <col min="35" max="35" width="13" customWidth="1"/>
-    <col min="36" max="36" width="20.1796875" customWidth="1"/>
-    <col min="37" max="37" width="18.81640625" customWidth="1"/>
-    <col min="38" max="38" width="16.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="11" width="14.1796875" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="64.1796875" customWidth="1"/>
+    <col min="15" max="15" width="16.36328125" customWidth="1"/>
+    <col min="16" max="21" width="21" customWidth="1"/>
+    <col min="22" max="22" width="21.90625" customWidth="1"/>
+    <col min="23" max="27" width="42.90625" customWidth="1"/>
+    <col min="28" max="29" width="14.36328125" customWidth="1"/>
+    <col min="32" max="32" width="13" customWidth="1"/>
+    <col min="33" max="33" width="20.1796875" customWidth="1"/>
+    <col min="34" max="34" width="18.81640625" customWidth="1"/>
+    <col min="35" max="35" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -615,106 +600,97 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG1" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>39</v>
-      </c>
       <c r="AH1" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="AI1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -733,86 +709,80 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" t="s">
         <v>5</v>
       </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
       <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="AB2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" t="s">
         <v>3</v>
       </c>
-      <c r="X2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AE2" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>15</v>
       </c>
-      <c r="AE2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>47</v>
-      </c>
       <c r="AG2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AH2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="AI2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -834,104 +804,104 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.13</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="P3" s="1">
         <v>0.13</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="1">
+        <v>137</v>
+      </c>
+      <c r="U3" s="1">
+        <v>137</v>
+      </c>
+      <c r="V3" s="1">
+        <v>435</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U3" s="2" t="s">
+      <c r="Y3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" s="1">
-        <v>137</v>
-      </c>
-      <c r="X3" s="1">
-        <v>137</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>435</v>
-      </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>0.18</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>65</v>
-      </c>
     </row>
-    <row r="4" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
first push ubp calculation
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walkerl\Documents\code\sia_380-1-full_version\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LW_Simulation\PycharmProjects\sia_380-1-full_version\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="9470"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Configuration</t>
   </si>
@@ -170,57 +179,18 @@
     <t>m-Si</t>
   </si>
   <si>
-    <t>UBA_EnEV_wall_stb</t>
-  </si>
-  <si>
-    <t>UBA_EnEV_roof_stb</t>
-  </si>
-  <si>
-    <t>UBA_EnEV_window</t>
-  </si>
-  <si>
-    <t>UBA_all_stb</t>
-  </si>
-  <si>
     <t>ceiling type</t>
   </si>
   <si>
-    <t>117.0 117.0 117.0 117.0</t>
-  </si>
-  <si>
-    <t>5.0 10.0 10.0 35.0</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>GSHP</t>
   </si>
   <si>
-    <t>ASHP</t>
-  </si>
-  <si>
     <t>increased ventilation volume flow</t>
   </si>
   <si>
-    <t>105 30</t>
-  </si>
-  <si>
-    <t>26 25</t>
-  </si>
-  <si>
-    <t>180 120</t>
-  </si>
-  <si>
     <t>cold emission system</t>
   </si>
   <si>
-    <t>air</t>
-  </si>
-  <si>
-    <t>radiator</t>
-  </si>
-  <si>
     <t>heat pump efficiency</t>
   </si>
   <si>
@@ -228,12 +198,39 @@
   </si>
   <si>
     <t>"same" or the choices from heating system</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>hydronic</t>
+  </si>
+  <si>
+    <t>floor heating</t>
+  </si>
+  <si>
+    <t>344.5 344.5 344.5 344.5</t>
+  </si>
+  <si>
+    <t>112.7 112.7 112.7 112.7</t>
+  </si>
+  <si>
+    <t>Wall_BC1</t>
+  </si>
+  <si>
+    <t>Roof_BC1</t>
+  </si>
+  <si>
+    <t>Window_BC1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,18 +240,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -269,10 +260,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,35 +548,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" customWidth="1"/>
-    <col min="3" max="3" width="30.90625" customWidth="1"/>
-    <col min="4" max="4" width="23.453125" customWidth="1"/>
-    <col min="5" max="6" width="22.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="11" width="14.1796875" customWidth="1"/>
-    <col min="12" max="12" width="14.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" customWidth="1"/>
-    <col min="14" max="14" width="64.1796875" customWidth="1"/>
-    <col min="15" max="15" width="16.36328125" customWidth="1"/>
+    <col min="9" max="11" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="64.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
     <col min="16" max="21" width="21" customWidth="1"/>
-    <col min="22" max="22" width="21.90625" customWidth="1"/>
-    <col min="23" max="27" width="42.90625" customWidth="1"/>
-    <col min="28" max="29" width="14.36328125" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" customWidth="1"/>
+    <col min="23" max="27" width="42.85546875" customWidth="1"/>
+    <col min="28" max="29" width="14.28515625" customWidth="1"/>
     <col min="32" max="32" width="13" customWidth="1"/>
-    <col min="33" max="33" width="20.1796875" customWidth="1"/>
-    <col min="34" max="34" width="18.81640625" customWidth="1"/>
-    <col min="35" max="35" width="16.6328125" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" customWidth="1"/>
+    <col min="34" max="34" width="18.85546875" customWidth="1"/>
+    <col min="35" max="35" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -612,7 +605,7 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
         <v>40</v>
@@ -654,7 +647,7 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="Y1" t="s">
         <v>42</v>
@@ -663,13 +656,13 @@
         <v>43</v>
       </c>
       <c r="AA1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="AB1" t="s">
         <v>35</v>
       </c>
       <c r="AC1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="AD1" t="s">
         <v>37</v>
@@ -690,7 +683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -746,7 +739,7 @@
         <v>19</v>
       </c>
       <c r="X2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="Y2" t="s">
         <v>44</v>
@@ -782,231 +775,239 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>520</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.215</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="B3" s="2">
+        <v>2966</v>
+      </c>
+      <c r="C3" s="2">
         <v>0.15</v>
       </c>
-      <c r="E3" s="1">
+      <c r="D3" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E3" s="4">
+        <f>4100/B3</f>
+        <v>1.3823331085637223</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.38</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="3">
+        <f>0.11*1068/(1068+310)+0.101*310/(1068+310)</f>
+        <v>0.10797532656023223</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="4">
+        <f>0.9*393/(393+58)+1.23*58/(393+58)</f>
+        <v>0.94243902439024385</v>
+      </c>
+      <c r="M3" s="4">
+        <f>0.6*393/(393+58)+1.1*58/(393+58)</f>
+        <v>0.66430155210643016</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="3">
+        <f>0.16*250/(250+460)+0.1*460/(250+460)</f>
+        <v>0.12112676056338029</v>
+      </c>
+      <c r="P3" s="3">
+        <f>0.16*242/(242+387)+0.28*387/(242+387)</f>
+        <v>0.23383147853736092</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="2">
+        <f>250+460</f>
+        <v>710</v>
+      </c>
+      <c r="U3" s="2">
+        <f>387+242</f>
+        <v>629</v>
+      </c>
+      <c r="V3" s="2">
+        <v>565</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="AE3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="1">
-        <v>137</v>
-      </c>
-      <c r="U3" s="1">
-        <v>137</v>
-      </c>
-      <c r="V3" s="1">
-        <v>435</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>0.18</v>
-      </c>
       <c r="AG3" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Zwischenspeichern push ubp calculation
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Configuration</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Window_BC1</t>
+  </si>
+  <si>
+    <t>Floor_BC1</t>
   </si>
 </sst>
 </file>
@@ -548,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +809,7 @@
         <v>0.10797532656023223</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>62</v>
@@ -887,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="AI3" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
General minor changes and cooling power monthly is not calculated anymore for cooling system == None
</commit_message>
<xml_diff>
--- a/data/configurations.xlsx
+++ b/data/configurations.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>Configuration</t>
   </si>
@@ -225,6 +225,21 @@
   </si>
   <si>
     <t>Floor_BC1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>thermal bridge add on</t>
+  </si>
+  <si>
+    <t>[%]</t>
+  </si>
+  <si>
+    <t>mechanical ventilation</t>
+  </si>
+  <si>
+    <t>True/False</t>
   </si>
 </sst>
 </file>
@@ -549,37 +564,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI121"/>
+  <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="64.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" customWidth="1"/>
-    <col min="16" max="21" width="21" customWidth="1"/>
-    <col min="22" max="22" width="21.85546875" customWidth="1"/>
-    <col min="23" max="27" width="42.85546875" customWidth="1"/>
-    <col min="28" max="29" width="14.28515625" customWidth="1"/>
-    <col min="32" max="32" width="13" customWidth="1"/>
-    <col min="33" max="33" width="20.140625" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" customWidth="1"/>
-    <col min="35" max="35" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="23" width="21" customWidth="1"/>
+    <col min="24" max="24" width="21.85546875" customWidth="1"/>
+    <col min="25" max="25" width="42.85546875" customWidth="1"/>
+    <col min="26" max="26" width="40.5703125" customWidth="1"/>
+    <col min="27" max="27" width="17.28515625" customWidth="1"/>
+    <col min="28" max="28" width="40.42578125" customWidth="1"/>
+    <col min="29" max="29" width="42.85546875" customWidth="1"/>
+    <col min="30" max="31" width="14.28515625" customWidth="1"/>
+    <col min="34" max="34" width="13" customWidth="1"/>
+    <col min="35" max="35" width="20.140625" customWidth="1"/>
+    <col min="36" max="36" width="18.85546875" customWidth="1"/>
+    <col min="37" max="37" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,94 +616,100 @@
         <v>50</v>
       </c>
       <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>32</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>33</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>22</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -703,82 +726,88 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>5</v>
       </c>
       <c r="P2" t="s">
         <v>5</v>
       </c>
       <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>27</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>29</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>3</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>3</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>19</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>44</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>3</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>47</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>15</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -792,120 +821,125 @@
         <v>0.15</v>
       </c>
       <c r="E3" s="4">
-        <f>4100/B3</f>
-        <v>1.3823331085637223</v>
+        <v>0.7</v>
       </c>
       <c r="F3" s="2">
         <v>1.38</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <f>0.11*1068/(1068+310)+0.101*310/(1068+310)</f>
         <v>0.10797532656023223</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="4">
+      <c r="M3" s="4">
         <f>0.9*393/(393+58)+1.23*58/(393+58)</f>
         <v>0.94243902439024385</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <f>0.6*393/(393+58)+1.1*58/(393+58)</f>
         <v>0.66430155210643016</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <f>0.16*250/(250+460)+0.1*460/(250+460)</f>
         <v>0.12112676056338029</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <f>0.16*242/(242+387)+0.28*387/(242+387)</f>
         <v>0.23383147853736092</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <f>250+460</f>
         <v>710</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <f>387+242</f>
         <v>629</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <v>565</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA3" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>0</v>
+      <c r="AC3" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="AF3" s="2">
         <v>0</v>
       </c>
-      <c r="AG3" s="2">
-        <v>0</v>
+      <c r="AG3" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="AH3" s="2">
         <v>0</v>
       </c>
       <c r="AI3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>